<commit_message>
Initial add for preprocessing program
</commit_message>
<xml_diff>
--- a/homework_2/dataset/mapped_availability.xlsx
+++ b/homework_2/dataset/mapped_availability.xlsx
@@ -1,30 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Repositories\csci-540\homework_2\dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Desktop\Repositories\csci-540\homework_2\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB5610D-61B4-4F7B-AD3D-881298B904F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18110"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="234">
   <si>
     <t>Dataset Two NEMS-G</t>
   </si>
@@ -320,9 +330,6 @@
     <t>Available beef 20%-30% fat</t>
   </si>
   <si>
-    <t>ground beef</t>
-  </si>
-  <si>
     <t>Q78_5</t>
   </si>
   <si>
@@ -476,12 +483,6 @@
     <t>Available beverages other regular soda</t>
   </si>
   <si>
-    <t>Q109_5</t>
-  </si>
-  <si>
-    <t>Available beverages water unflavored</t>
-  </si>
-  <si>
     <t>Q109_6</t>
   </si>
   <si>
@@ -570,12 +571,177 @@
   </si>
   <si>
     <t>Available cereal none</t>
+  </si>
+  <si>
+    <t>if (fieldList[3].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[4].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[5].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[6].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[15].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[16].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[17].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[18].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[19].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[20].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[21].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[22].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[23].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[24].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[86].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[87].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[88].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[89].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[90].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[91].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[92].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[93].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[94].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[95].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[155].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[156].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[157].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[158].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[172].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[173].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[174].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[175].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[205].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[206].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[207].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[208].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[271].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[272].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[273].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[274].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[275].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[303].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[304].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[305].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[306].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[308].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[309].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[335].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[336].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[347].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[348].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[359].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>if (fieldList[360].equals("1")) foods.add("skim milk");</t>
+  </si>
+  <si>
+    <t>ground beef (80% lean)</t>
+  </si>
+  <si>
+    <t>ground beef (75% lean, regular)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -886,26 +1052,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I66"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="3.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="3.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -931,7 +1097,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -959,8 +1125,15 @@
       <c r="I2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K2" t="s">
+        <v>179</v>
+      </c>
+      <c r="L2" t="str">
+        <f>SUBSTITUTE(K2,"skim milk",D2)</f>
+        <v>if (fieldList[3].equals("1")) foods.add("skim milk");</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -988,8 +1161,15 @@
       <c r="I3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K3" t="s">
+        <v>180</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" ref="L3:L65" si="0">SUBSTITUTE(K3,"skim milk",D3)</f>
+        <v>if (fieldList[4].equals("1")) foods.add("1% milk");</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1017,8 +1197,15 @@
       <c r="I4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K4" t="s">
+        <v>181</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[5].equals("1")) foods.add("2% milk");</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1046,8 +1233,15 @@
       <c r="I5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K5" t="s">
+        <v>182</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[6].equals("1")) foods.add("whole milk");</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1072,8 +1266,12 @@
       <c r="I6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="L6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1101,8 +1299,15 @@
       <c r="I7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K7" t="s">
+        <v>183</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[15].equals("1")) foods.add("banana");</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1130,8 +1335,15 @@
       <c r="I8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K8" t="s">
+        <v>184</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[16].equals("1")) foods.add("apple");</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1159,8 +1371,15 @@
       <c r="I9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K9" t="s">
+        <v>185</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[17].equals("1")) foods.add("orange");</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1188,8 +1407,15 @@
       <c r="I10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K10" t="s">
+        <v>186</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[18].equals("1")) foods.add("grape");</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1217,8 +1443,15 @@
       <c r="I11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K11" t="s">
+        <v>187</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[19].equals("1")) foods.add("cantaloupe");</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1246,8 +1479,15 @@
       <c r="I12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K12" t="s">
+        <v>188</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[20].equals("1")) foods.add("peach");</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1275,8 +1515,15 @@
       <c r="I13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K13" t="s">
+        <v>189</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[21].equals("1")) foods.add("strawberry");</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1304,8 +1551,15 @@
       <c r="I14" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K14" t="s">
+        <v>190</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[22].equals("1")) foods.add("honey dew melon");</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1333,8 +1587,15 @@
       <c r="I15" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K15" t="s">
+        <v>191</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[23].equals("1")) foods.add("watermelon");</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1362,8 +1623,15 @@
       <c r="I16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K16" t="s">
+        <v>192</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[24].equals("1")) foods.add("pear");</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1388,8 +1656,12 @@
       <c r="I17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="L17" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1417,8 +1689,15 @@
       <c r="I18" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K18" t="s">
+        <v>193</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[86].equals("1")) foods.add("carrot");</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1446,8 +1725,15 @@
       <c r="I19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K19" t="s">
+        <v>194</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[87].equals("1")) foods.add("tomatoe");</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1475,8 +1761,15 @@
       <c r="I20" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K20" t="s">
+        <v>195</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[88].equals("1")) foods.add("sweet potatoe");</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1504,8 +1797,15 @@
       <c r="I21" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K21" t="s">
+        <v>196</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[89].equals("1")) foods.add("broccoli");</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1533,8 +1833,15 @@
       <c r="I22" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K22" t="s">
+        <v>197</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[90].equals("1")) foods.add("lettuce");</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -1562,8 +1869,15 @@
       <c r="I23" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K23" t="s">
+        <v>198</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[91].equals("1")) foods.add("corn");</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1591,8 +1905,15 @@
       <c r="I24" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K24" t="s">
+        <v>199</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[92].equals("1")) foods.add("celery");</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1620,8 +1941,15 @@
       <c r="I25" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K25" t="s">
+        <v>200</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[93].equals("1")) foods.add("cucumber");</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -1649,8 +1977,15 @@
       <c r="I26" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K26" t="s">
+        <v>201</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[94].equals("1")) foods.add("cabbage");</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -1678,8 +2013,15 @@
       <c r="I27" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K27" t="s">
+        <v>202</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[95].equals("1")) foods.add("cauliflower");</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -1704,8 +2046,12 @@
       <c r="I28" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="L28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -1733,8 +2079,15 @@
       <c r="I29" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K29" t="s">
+        <v>203</v>
+      </c>
+      <c r="L29" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[155].equals("1")) foods.add("ground beef (95% lean)");</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -1762,8 +2115,15 @@
       <c r="I30" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K30" t="s">
+        <v>204</v>
+      </c>
+      <c r="L30" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[156].equals("1")) foods.add("ground beef (90% lean)");</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -1791,8 +2151,15 @@
       <c r="I31" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K31" t="s">
+        <v>205</v>
+      </c>
+      <c r="L31" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[157].equals("1")) foods.add("ground beef (85% lean)");</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -1803,966 +2170,1186 @@
         <v>97</v>
       </c>
       <c r="D32" t="s">
+        <v>232</v>
+      </c>
+      <c r="E32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32">
+        <v>255</v>
+      </c>
+      <c r="G32" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" t="s">
+        <v>6</v>
+      </c>
+      <c r="I32" t="s">
+        <v>5</v>
+      </c>
+      <c r="K32" t="s">
+        <v>206</v>
+      </c>
+      <c r="L32" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[158].equals("1")) foods.add("ground beef (80% lean)");</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" t="s">
+        <v>233</v>
+      </c>
+      <c r="E33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33">
+        <v>255</v>
+      </c>
+      <c r="G33" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" t="s">
+        <v>6</v>
+      </c>
+      <c r="I33" t="s">
+        <v>5</v>
+      </c>
+      <c r="K33" t="s">
+        <v>206</v>
+      </c>
+      <c r="L33" t="str">
+        <f t="shared" ref="L33" si="1">SUBSTITUTE(K33,"skim milk",D33)</f>
+        <v>if (fieldList[158].equals("1")) foods.add("ground beef (75% lean, regular)");</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" t="s">
         <v>98</v>
       </c>
-      <c r="E32" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32">
-        <v>255</v>
-      </c>
-      <c r="G32" t="s">
-        <v>11</v>
-      </c>
-      <c r="H32" t="s">
-        <v>6</v>
-      </c>
-      <c r="I32" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="C34" t="s">
         <v>99</v>
       </c>
-      <c r="C33" t="s">
+      <c r="E34" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34">
+        <v>255</v>
+      </c>
+      <c r="G34" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" t="s">
+        <v>6</v>
+      </c>
+      <c r="I34" t="s">
+        <v>5</v>
+      </c>
+      <c r="L34" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" t="s">
         <v>100</v>
       </c>
-      <c r="E33" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33">
-        <v>255</v>
-      </c>
-      <c r="G33" t="s">
-        <v>11</v>
-      </c>
-      <c r="H33" t="s">
-        <v>6</v>
-      </c>
-      <c r="I33" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="C35" t="s">
         <v>101</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D35" t="s">
         <v>102</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35">
+        <v>255</v>
+      </c>
+      <c r="G35" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" t="s">
+        <v>6</v>
+      </c>
+      <c r="I35" t="s">
+        <v>5</v>
+      </c>
+      <c r="K35" t="s">
+        <v>207</v>
+      </c>
+      <c r="L35" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[172].equals("1")) foods.add("hot dog");</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" t="s">
         <v>103</v>
       </c>
-      <c r="E34" t="s">
-        <v>10</v>
-      </c>
-      <c r="F34">
-        <v>255</v>
-      </c>
-      <c r="G34" t="s">
-        <v>11</v>
-      </c>
-      <c r="H34" t="s">
-        <v>6</v>
-      </c>
-      <c r="I34" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="C36" t="s">
         <v>104</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D36" t="s">
+        <v>102</v>
+      </c>
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36">
+        <v>255</v>
+      </c>
+      <c r="G36" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" t="s">
+        <v>6</v>
+      </c>
+      <c r="I36" t="s">
+        <v>5</v>
+      </c>
+      <c r="K36" t="s">
+        <v>208</v>
+      </c>
+      <c r="L36" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[173].equals("1")) foods.add("hot dog");</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" t="s">
         <v>105</v>
       </c>
-      <c r="D35" t="s">
-        <v>103</v>
-      </c>
-      <c r="E35" t="s">
-        <v>10</v>
-      </c>
-      <c r="F35">
-        <v>255</v>
-      </c>
-      <c r="G35" t="s">
-        <v>11</v>
-      </c>
-      <c r="H35" t="s">
-        <v>6</v>
-      </c>
-      <c r="I35" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="C37" t="s">
         <v>106</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D37" t="s">
         <v>107</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37">
+        <v>255</v>
+      </c>
+      <c r="G37" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" t="s">
+        <v>6</v>
+      </c>
+      <c r="I37" t="s">
+        <v>5</v>
+      </c>
+      <c r="K37" t="s">
+        <v>209</v>
+      </c>
+      <c r="L37" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[174].equals("1")) foods.add("low fat hot dog");</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" t="s">
         <v>108</v>
       </c>
-      <c r="E36" t="s">
-        <v>10</v>
-      </c>
-      <c r="F36">
-        <v>255</v>
-      </c>
-      <c r="G36" t="s">
-        <v>11</v>
-      </c>
-      <c r="H36" t="s">
-        <v>6</v>
-      </c>
-      <c r="I36" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="C38" t="s">
         <v>109</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D38" t="s">
+        <v>102</v>
+      </c>
+      <c r="E38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38">
+        <v>255</v>
+      </c>
+      <c r="G38" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" t="s">
+        <v>6</v>
+      </c>
+      <c r="I38" t="s">
+        <v>5</v>
+      </c>
+      <c r="K38" t="s">
+        <v>210</v>
+      </c>
+      <c r="L38" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[175].equals("1")) foods.add("hot dog");</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" t="s">
         <v>110</v>
       </c>
-      <c r="D37" t="s">
-        <v>103</v>
-      </c>
-      <c r="E37" t="s">
-        <v>10</v>
-      </c>
-      <c r="F37">
-        <v>255</v>
-      </c>
-      <c r="G37" t="s">
-        <v>11</v>
-      </c>
-      <c r="H37" t="s">
-        <v>6</v>
-      </c>
-      <c r="I37" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>0</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="C39" t="s">
         <v>111</v>
       </c>
-      <c r="C38" t="s">
+      <c r="E39" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39">
+        <v>255</v>
+      </c>
+      <c r="G39" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" t="s">
+        <v>6</v>
+      </c>
+      <c r="I39" t="s">
+        <v>5</v>
+      </c>
+      <c r="L39" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" t="s">
         <v>112</v>
       </c>
-      <c r="E38" t="s">
-        <v>10</v>
-      </c>
-      <c r="F38">
-        <v>255</v>
-      </c>
-      <c r="G38" t="s">
-        <v>11</v>
-      </c>
-      <c r="H38" t="s">
-        <v>6</v>
-      </c>
-      <c r="I38" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>0</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="C40" t="s">
         <v>113</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D40" t="s">
         <v>114</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E40" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40">
+        <v>255</v>
+      </c>
+      <c r="G40" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" t="s">
+        <v>6</v>
+      </c>
+      <c r="I40" t="s">
+        <v>5</v>
+      </c>
+      <c r="K40" t="s">
+        <v>211</v>
+      </c>
+      <c r="L40" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[205].equals("1")) foods.add("frozen meal");</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" t="s">
         <v>115</v>
       </c>
-      <c r="E39" t="s">
-        <v>10</v>
-      </c>
-      <c r="F39">
-        <v>255</v>
-      </c>
-      <c r="G39" t="s">
-        <v>11</v>
-      </c>
-      <c r="H39" t="s">
-        <v>6</v>
-      </c>
-      <c r="I39" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="C41" t="s">
         <v>116</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D41" t="s">
+        <v>114</v>
+      </c>
+      <c r="E41" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41">
+        <v>255</v>
+      </c>
+      <c r="G41" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" t="s">
+        <v>6</v>
+      </c>
+      <c r="I41" t="s">
+        <v>5</v>
+      </c>
+      <c r="K41" t="s">
+        <v>212</v>
+      </c>
+      <c r="L41" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[206].equals("1")) foods.add("frozen meal");</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" t="s">
         <v>117</v>
       </c>
-      <c r="D40" t="s">
-        <v>115</v>
-      </c>
-      <c r="E40" t="s">
-        <v>10</v>
-      </c>
-      <c r="F40">
-        <v>255</v>
-      </c>
-      <c r="G40" t="s">
-        <v>11</v>
-      </c>
-      <c r="H40" t="s">
-        <v>6</v>
-      </c>
-      <c r="I40" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>0</v>
-      </c>
-      <c r="B41" t="s">
+      <c r="C42" t="s">
         <v>118</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D42" t="s">
+        <v>114</v>
+      </c>
+      <c r="E42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42">
+        <v>255</v>
+      </c>
+      <c r="G42" t="s">
+        <v>11</v>
+      </c>
+      <c r="H42" t="s">
+        <v>6</v>
+      </c>
+      <c r="I42" t="s">
+        <v>5</v>
+      </c>
+      <c r="K42" t="s">
+        <v>213</v>
+      </c>
+      <c r="L42" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[207].equals("1")) foods.add("frozen meal");</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" t="s">
         <v>119</v>
       </c>
-      <c r="D41" t="s">
-        <v>115</v>
-      </c>
-      <c r="E41" t="s">
-        <v>10</v>
-      </c>
-      <c r="F41">
-        <v>255</v>
-      </c>
-      <c r="G41" t="s">
-        <v>11</v>
-      </c>
-      <c r="H41" t="s">
-        <v>6</v>
-      </c>
-      <c r="I41" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>0</v>
-      </c>
-      <c r="B42" t="s">
+      <c r="C43" t="s">
         <v>120</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D43" t="s">
+        <v>114</v>
+      </c>
+      <c r="E43" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43">
+        <v>255</v>
+      </c>
+      <c r="G43" t="s">
+        <v>11</v>
+      </c>
+      <c r="H43" t="s">
+        <v>6</v>
+      </c>
+      <c r="I43" t="s">
+        <v>5</v>
+      </c>
+      <c r="K43" t="s">
+        <v>214</v>
+      </c>
+      <c r="L43" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[208].equals("1")) foods.add("frozen meal");</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" t="s">
         <v>121</v>
       </c>
-      <c r="D42" t="s">
-        <v>115</v>
-      </c>
-      <c r="E42" t="s">
-        <v>10</v>
-      </c>
-      <c r="F42">
-        <v>255</v>
-      </c>
-      <c r="G42" t="s">
-        <v>11</v>
-      </c>
-      <c r="H42" t="s">
-        <v>6</v>
-      </c>
-      <c r="I42" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>0</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="C44" t="s">
         <v>122</v>
       </c>
-      <c r="C43" t="s">
+      <c r="E44" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44">
+        <v>255</v>
+      </c>
+      <c r="G44" t="s">
+        <v>11</v>
+      </c>
+      <c r="H44" t="s">
+        <v>6</v>
+      </c>
+      <c r="I44" t="s">
+        <v>5</v>
+      </c>
+      <c r="L44" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" t="s">
         <v>123</v>
       </c>
-      <c r="E43" t="s">
-        <v>10</v>
-      </c>
-      <c r="F43">
-        <v>255</v>
-      </c>
-      <c r="G43" t="s">
-        <v>11</v>
-      </c>
-      <c r="H43" t="s">
-        <v>6</v>
-      </c>
-      <c r="I43" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>0</v>
-      </c>
-      <c r="B44" t="s">
+      <c r="C45" t="s">
         <v>124</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D45" t="s">
         <v>125</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E45" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45">
+        <v>255</v>
+      </c>
+      <c r="G45" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45" t="s">
+        <v>6</v>
+      </c>
+      <c r="I45" t="s">
+        <v>5</v>
+      </c>
+      <c r="K45" t="s">
+        <v>215</v>
+      </c>
+      <c r="L45" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[271].equals("1")) foods.add("bagel");</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" t="s">
         <v>126</v>
       </c>
-      <c r="E44" t="s">
-        <v>10</v>
-      </c>
-      <c r="F44">
-        <v>255</v>
-      </c>
-      <c r="G44" t="s">
-        <v>11</v>
-      </c>
-      <c r="H44" t="s">
-        <v>6</v>
-      </c>
-      <c r="I44" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>0</v>
-      </c>
-      <c r="B45" t="s">
+      <c r="C46" t="s">
         <v>127</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D46" t="s">
         <v>128</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E46" t="s">
+        <v>10</v>
+      </c>
+      <c r="F46">
+        <v>255</v>
+      </c>
+      <c r="G46" t="s">
+        <v>11</v>
+      </c>
+      <c r="H46" t="s">
+        <v>6</v>
+      </c>
+      <c r="I46" t="s">
+        <v>5</v>
+      </c>
+      <c r="K46" t="s">
+        <v>216</v>
+      </c>
+      <c r="L46" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[272].equals("1")) foods.add("english muffin");</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" t="s">
         <v>129</v>
       </c>
-      <c r="E45" t="s">
-        <v>10</v>
-      </c>
-      <c r="F45">
-        <v>255</v>
-      </c>
-      <c r="G45" t="s">
-        <v>11</v>
-      </c>
-      <c r="H45" t="s">
-        <v>6</v>
-      </c>
-      <c r="I45" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>0</v>
-      </c>
-      <c r="B46" t="s">
+      <c r="C47" t="s">
         <v>130</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D47" t="s">
         <v>131</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47">
+        <v>255</v>
+      </c>
+      <c r="G47" t="s">
+        <v>11</v>
+      </c>
+      <c r="H47" t="s">
+        <v>6</v>
+      </c>
+      <c r="I47" t="s">
+        <v>5</v>
+      </c>
+      <c r="K47" t="s">
+        <v>217</v>
+      </c>
+      <c r="L47" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[273].equals("1")) foods.add("muffin");</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" t="s">
         <v>132</v>
       </c>
-      <c r="E46" t="s">
-        <v>10</v>
-      </c>
-      <c r="F46">
-        <v>255</v>
-      </c>
-      <c r="G46" t="s">
-        <v>11</v>
-      </c>
-      <c r="H46" t="s">
-        <v>6</v>
-      </c>
-      <c r="I46" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" t="s">
+      <c r="C48" t="s">
         <v>133</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D48" t="s">
+        <v>131</v>
+      </c>
+      <c r="E48" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48">
+        <v>255</v>
+      </c>
+      <c r="G48" t="s">
+        <v>11</v>
+      </c>
+      <c r="H48" t="s">
+        <v>6</v>
+      </c>
+      <c r="I48" t="s">
+        <v>5</v>
+      </c>
+      <c r="K48" t="s">
+        <v>218</v>
+      </c>
+      <c r="L48" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[274].equals("1")) foods.add("muffin");</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" t="s">
         <v>134</v>
       </c>
-      <c r="D47" t="s">
-        <v>132</v>
-      </c>
-      <c r="E47" t="s">
-        <v>10</v>
-      </c>
-      <c r="F47">
-        <v>255</v>
-      </c>
-      <c r="G47" t="s">
-        <v>11</v>
-      </c>
-      <c r="H47" t="s">
-        <v>6</v>
-      </c>
-      <c r="I47" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>0</v>
-      </c>
-      <c r="B48" t="s">
+      <c r="C49" t="s">
         <v>135</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D49" t="s">
         <v>136</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E49" t="s">
+        <v>10</v>
+      </c>
+      <c r="F49">
+        <v>255</v>
+      </c>
+      <c r="G49" t="s">
+        <v>11</v>
+      </c>
+      <c r="H49" t="s">
+        <v>6</v>
+      </c>
+      <c r="I49" t="s">
+        <v>5</v>
+      </c>
+      <c r="K49" t="s">
+        <v>219</v>
+      </c>
+      <c r="L49" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[275].equals("1")) foods.add("danish");</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" t="s">
         <v>137</v>
       </c>
-      <c r="E48" t="s">
-        <v>10</v>
-      </c>
-      <c r="F48">
-        <v>255</v>
-      </c>
-      <c r="G48" t="s">
-        <v>11</v>
-      </c>
-      <c r="H48" t="s">
-        <v>6</v>
-      </c>
-      <c r="I48" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>0</v>
-      </c>
-      <c r="B49" t="s">
+      <c r="C50" t="s">
         <v>138</v>
       </c>
-      <c r="C49" t="s">
+      <c r="E50" t="s">
+        <v>10</v>
+      </c>
+      <c r="F50">
+        <v>255</v>
+      </c>
+      <c r="G50" t="s">
+        <v>11</v>
+      </c>
+      <c r="H50" t="s">
+        <v>6</v>
+      </c>
+      <c r="I50" t="s">
+        <v>5</v>
+      </c>
+      <c r="L50" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" t="s">
         <v>139</v>
       </c>
-      <c r="E49" t="s">
-        <v>10</v>
-      </c>
-      <c r="F49">
-        <v>255</v>
-      </c>
-      <c r="G49" t="s">
-        <v>11</v>
-      </c>
-      <c r="H49" t="s">
-        <v>6</v>
-      </c>
-      <c r="I49" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>0</v>
-      </c>
-      <c r="B50" t="s">
+      <c r="C51" t="s">
         <v>140</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D51" t="s">
         <v>141</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E51" t="s">
+        <v>10</v>
+      </c>
+      <c r="F51">
+        <v>255</v>
+      </c>
+      <c r="G51" t="s">
+        <v>11</v>
+      </c>
+      <c r="H51" t="s">
+        <v>6</v>
+      </c>
+      <c r="I51" t="s">
+        <v>5</v>
+      </c>
+      <c r="K51" t="s">
+        <v>220</v>
+      </c>
+      <c r="L51" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[303].equals("1")) foods.add("soft drink, diet");</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" t="s">
         <v>142</v>
       </c>
-      <c r="E50" t="s">
-        <v>10</v>
-      </c>
-      <c r="F50">
-        <v>255</v>
-      </c>
-      <c r="G50" t="s">
-        <v>11</v>
-      </c>
-      <c r="H50" t="s">
-        <v>6</v>
-      </c>
-      <c r="I50" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>0</v>
-      </c>
-      <c r="B51" t="s">
+      <c r="C52" t="s">
         <v>143</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D52" t="s">
+        <v>141</v>
+      </c>
+      <c r="E52" t="s">
+        <v>10</v>
+      </c>
+      <c r="F52">
+        <v>255</v>
+      </c>
+      <c r="G52" t="s">
+        <v>11</v>
+      </c>
+      <c r="H52" t="s">
+        <v>6</v>
+      </c>
+      <c r="I52" t="s">
+        <v>5</v>
+      </c>
+      <c r="K52" t="s">
+        <v>221</v>
+      </c>
+      <c r="L52" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[304].equals("1")) foods.add("soft drink, diet");</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" t="s">
         <v>144</v>
       </c>
-      <c r="D51" t="s">
-        <v>142</v>
-      </c>
-      <c r="E51" t="s">
-        <v>10</v>
-      </c>
-      <c r="F51">
-        <v>255</v>
-      </c>
-      <c r="G51" t="s">
-        <v>11</v>
-      </c>
-      <c r="H51" t="s">
-        <v>6</v>
-      </c>
-      <c r="I51" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>0</v>
-      </c>
-      <c r="B52" t="s">
+      <c r="C53" t="s">
         <v>145</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D53" t="s">
         <v>146</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E53" t="s">
+        <v>10</v>
+      </c>
+      <c r="F53">
+        <v>255</v>
+      </c>
+      <c r="G53" t="s">
+        <v>11</v>
+      </c>
+      <c r="H53" t="s">
+        <v>6</v>
+      </c>
+      <c r="I53" t="s">
+        <v>5</v>
+      </c>
+      <c r="K53" t="s">
+        <v>222</v>
+      </c>
+      <c r="L53" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[305].equals("1")) foods.add("soft drink, regular");</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" t="s">
         <v>147</v>
       </c>
-      <c r="E52" t="s">
-        <v>10</v>
-      </c>
-      <c r="F52">
-        <v>255</v>
-      </c>
-      <c r="G52" t="s">
-        <v>11</v>
-      </c>
-      <c r="H52" t="s">
-        <v>6</v>
-      </c>
-      <c r="I52" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>0</v>
-      </c>
-      <c r="B53" t="s">
+      <c r="C54" t="s">
         <v>148</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D54" t="s">
+        <v>146</v>
+      </c>
+      <c r="E54" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54">
+        <v>255</v>
+      </c>
+      <c r="G54" t="s">
+        <v>11</v>
+      </c>
+      <c r="H54" t="s">
+        <v>6</v>
+      </c>
+      <c r="I54" t="s">
+        <v>5</v>
+      </c>
+      <c r="K54" t="s">
+        <v>223</v>
+      </c>
+      <c r="L54" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[306].equals("1")) foods.add("soft drink, regular");</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" t="s">
         <v>149</v>
       </c>
-      <c r="D53" t="s">
-        <v>147</v>
-      </c>
-      <c r="E53" t="s">
-        <v>10</v>
-      </c>
-      <c r="F53">
-        <v>255</v>
-      </c>
-      <c r="G53" t="s">
-        <v>11</v>
-      </c>
-      <c r="H53" t="s">
-        <v>6</v>
-      </c>
-      <c r="I53" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>0</v>
-      </c>
-      <c r="B54" t="s">
+      <c r="C55" t="s">
         <v>150</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D55" t="s">
         <v>151</v>
       </c>
-      <c r="E54" t="s">
-        <v>10</v>
-      </c>
-      <c r="F54">
-        <v>255</v>
-      </c>
-      <c r="G54" t="s">
-        <v>11</v>
-      </c>
-      <c r="H54" t="s">
-        <v>6</v>
-      </c>
-      <c r="I54" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>0</v>
-      </c>
-      <c r="B55" t="s">
+      <c r="E55" t="s">
+        <v>10</v>
+      </c>
+      <c r="F55">
+        <v>255</v>
+      </c>
+      <c r="G55" t="s">
+        <v>11</v>
+      </c>
+      <c r="H55" t="s">
+        <v>6</v>
+      </c>
+      <c r="I55" t="s">
+        <v>5</v>
+      </c>
+      <c r="K55" t="s">
+        <v>224</v>
+      </c>
+      <c r="L55" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[308].equals("1")) foods.add("100% juice");</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" t="s">
         <v>152</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C56" t="s">
         <v>153</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D56" t="s">
         <v>154</v>
       </c>
-      <c r="E55" t="s">
-        <v>10</v>
-      </c>
-      <c r="F55">
-        <v>255</v>
-      </c>
-      <c r="G55" t="s">
-        <v>11</v>
-      </c>
-      <c r="H55" t="s">
-        <v>6</v>
-      </c>
-      <c r="I55" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>0</v>
-      </c>
-      <c r="B56" t="s">
+      <c r="E56" t="s">
+        <v>10</v>
+      </c>
+      <c r="F56">
+        <v>255</v>
+      </c>
+      <c r="G56" t="s">
+        <v>11</v>
+      </c>
+      <c r="H56" t="s">
+        <v>6</v>
+      </c>
+      <c r="I56" t="s">
+        <v>5</v>
+      </c>
+      <c r="K56" t="s">
+        <v>225</v>
+      </c>
+      <c r="L56" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[309].equals("1")) foods.add("juice");</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" t="s">
         <v>155</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>156</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E57" t="s">
+        <v>10</v>
+      </c>
+      <c r="F57">
+        <v>255</v>
+      </c>
+      <c r="G57" t="s">
+        <v>11</v>
+      </c>
+      <c r="H57" t="s">
+        <v>6</v>
+      </c>
+      <c r="I57" t="s">
+        <v>5</v>
+      </c>
+      <c r="L57" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" t="s">
         <v>157</v>
       </c>
-      <c r="E56" t="s">
-        <v>10</v>
-      </c>
-      <c r="F56">
-        <v>255</v>
-      </c>
-      <c r="G56" t="s">
-        <v>11</v>
-      </c>
-      <c r="H56" t="s">
-        <v>6</v>
-      </c>
-      <c r="I56" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>0</v>
-      </c>
-      <c r="B57" t="s">
+      <c r="C58" t="s">
         <v>158</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D58" t="s">
         <v>159</v>
       </c>
-      <c r="E57" t="s">
-        <v>10</v>
-      </c>
-      <c r="F57">
-        <v>255</v>
-      </c>
-      <c r="G57" t="s">
-        <v>11</v>
-      </c>
-      <c r="H57" t="s">
-        <v>6</v>
-      </c>
-      <c r="I57" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>0</v>
-      </c>
-      <c r="B58" t="s">
+      <c r="E58" t="s">
+        <v>10</v>
+      </c>
+      <c r="F58">
+        <v>255</v>
+      </c>
+      <c r="G58" t="s">
+        <v>11</v>
+      </c>
+      <c r="H58" t="s">
+        <v>6</v>
+      </c>
+      <c r="I58" t="s">
+        <v>5</v>
+      </c>
+      <c r="K58" t="s">
+        <v>226</v>
+      </c>
+      <c r="L58" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[335].equals("1")) foods.add("whole wheat bread");</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" t="s">
         <v>160</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>161</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D59" t="s">
         <v>162</v>
       </c>
-      <c r="E58" t="s">
-        <v>10</v>
-      </c>
-      <c r="F58">
-        <v>255</v>
-      </c>
-      <c r="G58" t="s">
-        <v>11</v>
-      </c>
-      <c r="H58" t="s">
-        <v>6</v>
-      </c>
-      <c r="I58" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>0</v>
-      </c>
-      <c r="B59" t="s">
+      <c r="E59" t="s">
+        <v>10</v>
+      </c>
+      <c r="F59">
+        <v>255</v>
+      </c>
+      <c r="G59" t="s">
+        <v>11</v>
+      </c>
+      <c r="H59" t="s">
+        <v>6</v>
+      </c>
+      <c r="I59" t="s">
+        <v>5</v>
+      </c>
+      <c r="K59" t="s">
+        <v>227</v>
+      </c>
+      <c r="L59" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[336].equals("1")) foods.add("white bread");</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" t="s">
         <v>163</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C60" t="s">
         <v>164</v>
       </c>
-      <c r="D59" t="s">
+      <c r="E60" t="s">
+        <v>10</v>
+      </c>
+      <c r="F60">
+        <v>255</v>
+      </c>
+      <c r="G60" t="s">
+        <v>11</v>
+      </c>
+      <c r="H60" t="s">
+        <v>6</v>
+      </c>
+      <c r="I60" t="s">
+        <v>5</v>
+      </c>
+      <c r="L60" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" t="s">
         <v>165</v>
       </c>
-      <c r="E59" t="s">
-        <v>10</v>
-      </c>
-      <c r="F59">
-        <v>255</v>
-      </c>
-      <c r="G59" t="s">
-        <v>11</v>
-      </c>
-      <c r="H59" t="s">
-        <v>6</v>
-      </c>
-      <c r="I59" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>0</v>
-      </c>
-      <c r="B60" t="s">
+      <c r="C61" t="s">
         <v>166</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D61" t="s">
         <v>167</v>
       </c>
-      <c r="E60" t="s">
-        <v>10</v>
-      </c>
-      <c r="F60">
-        <v>255</v>
-      </c>
-      <c r="G60" t="s">
-        <v>11</v>
-      </c>
-      <c r="H60" t="s">
-        <v>6</v>
-      </c>
-      <c r="I60" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>0</v>
-      </c>
-      <c r="B61" t="s">
+      <c r="E61" t="s">
+        <v>10</v>
+      </c>
+      <c r="F61">
+        <v>255</v>
+      </c>
+      <c r="G61" t="s">
+        <v>11</v>
+      </c>
+      <c r="H61" t="s">
+        <v>6</v>
+      </c>
+      <c r="I61" t="s">
+        <v>5</v>
+      </c>
+      <c r="K61" t="s">
+        <v>228</v>
+      </c>
+      <c r="L61" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[347].equals("1")) foods.add("chips");</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>0</v>
+      </c>
+      <c r="B62" t="s">
         <v>168</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C62" t="s">
         <v>169</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D62" t="s">
+        <v>167</v>
+      </c>
+      <c r="E62" t="s">
+        <v>10</v>
+      </c>
+      <c r="F62">
+        <v>255</v>
+      </c>
+      <c r="G62" t="s">
+        <v>11</v>
+      </c>
+      <c r="H62" t="s">
+        <v>6</v>
+      </c>
+      <c r="I62" t="s">
+        <v>5</v>
+      </c>
+      <c r="K62" t="s">
+        <v>229</v>
+      </c>
+      <c r="L62" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[348].equals("1")) foods.add("chips");</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63" t="s">
         <v>170</v>
       </c>
-      <c r="E61" t="s">
-        <v>10</v>
-      </c>
-      <c r="F61">
-        <v>255</v>
-      </c>
-      <c r="G61" t="s">
-        <v>11</v>
-      </c>
-      <c r="H61" t="s">
-        <v>6</v>
-      </c>
-      <c r="I61" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>0</v>
-      </c>
-      <c r="B62" t="s">
+      <c r="C63" t="s">
         <v>171</v>
       </c>
-      <c r="C62" t="s">
+      <c r="E63" t="s">
+        <v>10</v>
+      </c>
+      <c r="F63">
+        <v>255</v>
+      </c>
+      <c r="G63" t="s">
+        <v>11</v>
+      </c>
+      <c r="H63" t="s">
+        <v>6</v>
+      </c>
+      <c r="I63" t="s">
+        <v>5</v>
+      </c>
+      <c r="L63" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" t="s">
         <v>172</v>
       </c>
-      <c r="D62" t="s">
-        <v>170</v>
-      </c>
-      <c r="E62" t="s">
-        <v>10</v>
-      </c>
-      <c r="F62">
-        <v>255</v>
-      </c>
-      <c r="G62" t="s">
-        <v>11</v>
-      </c>
-      <c r="H62" t="s">
-        <v>6</v>
-      </c>
-      <c r="I62" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>0</v>
-      </c>
-      <c r="B63" t="s">
+      <c r="C64" t="s">
         <v>173</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D64" t="s">
         <v>174</v>
       </c>
-      <c r="E63" t="s">
-        <v>10</v>
-      </c>
-      <c r="F63">
-        <v>255</v>
-      </c>
-      <c r="G63" t="s">
-        <v>11</v>
-      </c>
-      <c r="H63" t="s">
-        <v>6</v>
-      </c>
-      <c r="I63" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>0</v>
-      </c>
-      <c r="B64" t="s">
+      <c r="E64" t="s">
+        <v>10</v>
+      </c>
+      <c r="F64">
+        <v>255</v>
+      </c>
+      <c r="G64" t="s">
+        <v>11</v>
+      </c>
+      <c r="H64" t="s">
+        <v>6</v>
+      </c>
+      <c r="I64" t="s">
+        <v>5</v>
+      </c>
+      <c r="K64" t="s">
+        <v>230</v>
+      </c>
+      <c r="L64" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[359].equals("1")) foods.add("cereal");</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>0</v>
+      </c>
+      <c r="B65" t="s">
         <v>175</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C65" t="s">
         <v>176</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D65" t="s">
+        <v>174</v>
+      </c>
+      <c r="E65" t="s">
+        <v>10</v>
+      </c>
+      <c r="F65">
+        <v>255</v>
+      </c>
+      <c r="G65" t="s">
+        <v>11</v>
+      </c>
+      <c r="H65" t="s">
+        <v>6</v>
+      </c>
+      <c r="I65" t="s">
+        <v>5</v>
+      </c>
+      <c r="K65" t="s">
+        <v>231</v>
+      </c>
+      <c r="L65" t="str">
+        <f t="shared" si="0"/>
+        <v>if (fieldList[360].equals("1")) foods.add("cereal");</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>0</v>
+      </c>
+      <c r="B66" t="s">
         <v>177</v>
       </c>
-      <c r="E64" t="s">
-        <v>10</v>
-      </c>
-      <c r="F64">
-        <v>255</v>
-      </c>
-      <c r="G64" t="s">
-        <v>11</v>
-      </c>
-      <c r="H64" t="s">
-        <v>6</v>
-      </c>
-      <c r="I64" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>0</v>
-      </c>
-      <c r="B65" t="s">
+      <c r="C66" t="s">
         <v>178</v>
-      </c>
-      <c r="C65" t="s">
-        <v>179</v>
-      </c>
-      <c r="D65" t="s">
-        <v>177</v>
-      </c>
-      <c r="E65" t="s">
-        <v>10</v>
-      </c>
-      <c r="F65">
-        <v>255</v>
-      </c>
-      <c r="G65" t="s">
-        <v>11</v>
-      </c>
-      <c r="H65" t="s">
-        <v>6</v>
-      </c>
-      <c r="I65" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>0</v>
-      </c>
-      <c r="B66" t="s">
-        <v>180</v>
-      </c>
-      <c r="C66" t="s">
-        <v>181</v>
       </c>
       <c r="E66" t="s">
         <v>10</v>
@@ -2782,5 +3369,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Rework preprocessing to use a hashmap to prevent duplicate values
</commit_message>
<xml_diff>
--- a/homework_2/dataset/mapped_availability.xlsx
+++ b/homework_2/dataset/mapped_availability.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Desktop\Repositories\csci-540\homework_2\dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Repositories\csci-540\homework_2\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB5610D-61B4-4F7B-AD3D-881298B904F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -573,175 +572,175 @@
     <t>Available cereal none</t>
   </si>
   <si>
-    <t>if (fieldList[3].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[4].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[5].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[6].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[15].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[16].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[17].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[18].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[19].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[20].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[21].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[22].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[23].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[24].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[86].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[87].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[88].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[89].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[90].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[91].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[92].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[93].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[94].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[95].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[155].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[156].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[157].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[158].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[172].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[173].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[174].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[175].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[205].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[206].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[207].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[208].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[271].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[272].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[273].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[274].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[275].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[303].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[304].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[305].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[306].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[308].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[309].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[335].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[336].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[347].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[348].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[359].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
-    <t>if (fieldList[360].equals("1")) foods.add("skim milk");</t>
-  </si>
-  <si>
     <t>ground beef (80% lean)</t>
   </si>
   <si>
     <t>ground beef (75% lean, regular)</t>
+  </si>
+  <si>
+    <t>if (fieldList[3].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[4].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[5].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[6].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[15].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[16].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[17].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[18].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[19].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[20].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[21].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[22].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[23].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[24].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[86].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[87].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[88].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[89].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[90].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[91].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[92].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[93].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[94].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[95].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[155].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[156].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[157].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[158].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[172].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[173].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[174].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[175].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[205].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[206].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[207].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[208].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[271].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[272].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[273].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[274].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[275].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[303].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[304].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[305].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[306].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[308].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[309].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[335].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[336].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[347].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[348].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[359].equals("1")) foods.put("skim milk", 1);</t>
+  </si>
+  <si>
+    <t>if (fieldList[360].equals("1")) foods.put("skim milk", 1);</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1052,26 +1051,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="Z33" sqref="Z33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="3.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1097,7 +1096,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1126,14 +1125,14 @@
         <v>5</v>
       </c>
       <c r="K2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="L2" t="str">
         <f>SUBSTITUTE(K2,"skim milk",D2)</f>
-        <v>if (fieldList[3].equals("1")) foods.add("skim milk");</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[3].equals("1")) foods.put("skim milk", 1);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1162,14 +1161,14 @@
         <v>5</v>
       </c>
       <c r="K3" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="L3" t="str">
         <f t="shared" ref="L3:L65" si="0">SUBSTITUTE(K3,"skim milk",D3)</f>
-        <v>if (fieldList[4].equals("1")) foods.add("1% milk");</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[4].equals("1")) foods.put("1% milk", 1);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1198,14 +1197,14 @@
         <v>5</v>
       </c>
       <c r="K4" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[5].equals("1")) foods.add("2% milk");</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[5].equals("1")) foods.put("2% milk", 1);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1234,14 +1233,14 @@
         <v>5</v>
       </c>
       <c r="K5" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[6].equals("1")) foods.add("whole milk");</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[6].equals("1")) foods.put("whole milk", 1);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1271,7 +1270,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1300,14 +1299,14 @@
         <v>5</v>
       </c>
       <c r="K7" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[15].equals("1")) foods.add("banana");</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[15].equals("1")) foods.put("banana", 1);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1336,14 +1335,14 @@
         <v>5</v>
       </c>
       <c r="K8" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[16].equals("1")) foods.add("apple");</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[16].equals("1")) foods.put("apple", 1);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1372,14 +1371,14 @@
         <v>5</v>
       </c>
       <c r="K9" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[17].equals("1")) foods.add("orange");</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[17].equals("1")) foods.put("orange", 1);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1408,14 +1407,14 @@
         <v>5</v>
       </c>
       <c r="K10" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[18].equals("1")) foods.add("grape");</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[18].equals("1")) foods.put("grape", 1);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1444,14 +1443,14 @@
         <v>5</v>
       </c>
       <c r="K11" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[19].equals("1")) foods.add("cantaloupe");</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[19].equals("1")) foods.put("cantaloupe", 1);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1480,14 +1479,14 @@
         <v>5</v>
       </c>
       <c r="K12" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[20].equals("1")) foods.add("peach");</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[20].equals("1")) foods.put("peach", 1);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1516,14 +1515,14 @@
         <v>5</v>
       </c>
       <c r="K13" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[21].equals("1")) foods.add("strawberry");</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[21].equals("1")) foods.put("strawberry", 1);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1552,14 +1551,14 @@
         <v>5</v>
       </c>
       <c r="K14" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[22].equals("1")) foods.add("honey dew melon");</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[22].equals("1")) foods.put("honey dew melon", 1);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1588,14 +1587,14 @@
         <v>5</v>
       </c>
       <c r="K15" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[23].equals("1")) foods.add("watermelon");</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[23].equals("1")) foods.put("watermelon", 1);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1624,14 +1623,14 @@
         <v>5</v>
       </c>
       <c r="K16" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[24].equals("1")) foods.add("pear");</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[24].equals("1")) foods.put("pear", 1);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1661,7 +1660,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1690,14 +1689,14 @@
         <v>5</v>
       </c>
       <c r="K18" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[86].equals("1")) foods.add("carrot");</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[86].equals("1")) foods.put("carrot", 1);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1726,14 +1725,14 @@
         <v>5</v>
       </c>
       <c r="K19" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[87].equals("1")) foods.add("tomatoe");</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[87].equals("1")) foods.put("tomatoe", 1);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1762,14 +1761,14 @@
         <v>5</v>
       </c>
       <c r="K20" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[88].equals("1")) foods.add("sweet potatoe");</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[88].equals("1")) foods.put("sweet potatoe", 1);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1798,14 +1797,14 @@
         <v>5</v>
       </c>
       <c r="K21" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[89].equals("1")) foods.add("broccoli");</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[89].equals("1")) foods.put("broccoli", 1);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1834,14 +1833,14 @@
         <v>5</v>
       </c>
       <c r="K22" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[90].equals("1")) foods.add("lettuce");</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[90].equals("1")) foods.put("lettuce", 1);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -1870,14 +1869,14 @@
         <v>5</v>
       </c>
       <c r="K23" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[91].equals("1")) foods.add("corn");</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[91].equals("1")) foods.put("corn", 1);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1906,14 +1905,14 @@
         <v>5</v>
       </c>
       <c r="K24" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[92].equals("1")) foods.add("celery");</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[92].equals("1")) foods.put("celery", 1);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1942,14 +1941,14 @@
         <v>5</v>
       </c>
       <c r="K25" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="L25" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[93].equals("1")) foods.add("cucumber");</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[93].equals("1")) foods.put("cucumber", 1);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -1978,14 +1977,14 @@
         <v>5</v>
       </c>
       <c r="K26" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="L26" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[94].equals("1")) foods.add("cabbage");</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[94].equals("1")) foods.put("cabbage", 1);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -2014,14 +2013,14 @@
         <v>5</v>
       </c>
       <c r="K27" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="L27" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[95].equals("1")) foods.add("cauliflower");</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[95].equals("1")) foods.put("cauliflower", 1);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -2051,7 +2050,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -2080,14 +2079,14 @@
         <v>5</v>
       </c>
       <c r="K29" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="L29" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[155].equals("1")) foods.add("ground beef (95% lean)");</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[155].equals("1")) foods.put("ground beef (95% lean)", 1);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -2116,14 +2115,14 @@
         <v>5</v>
       </c>
       <c r="K30" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="L30" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[156].equals("1")) foods.add("ground beef (90% lean)");</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[156].equals("1")) foods.put("ground beef (90% lean)", 1);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -2152,14 +2151,14 @@
         <v>5</v>
       </c>
       <c r="K31" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="L31" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[157].equals("1")) foods.add("ground beef (85% lean)");</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[157].equals("1")) foods.put("ground beef (85% lean)", 1);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -2170,7 +2169,7 @@
         <v>97</v>
       </c>
       <c r="D32" t="s">
-        <v>232</v>
+        <v>179</v>
       </c>
       <c r="E32" t="s">
         <v>10</v>
@@ -2188,14 +2187,14 @@
         <v>5</v>
       </c>
       <c r="K32" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="L32" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[158].equals("1")) foods.add("ground beef (80% lean)");</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[158].equals("1")) foods.put("ground beef (80% lean)", 1);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -2206,7 +2205,7 @@
         <v>97</v>
       </c>
       <c r="D33" t="s">
-        <v>233</v>
+        <v>180</v>
       </c>
       <c r="E33" t="s">
         <v>10</v>
@@ -2224,14 +2223,14 @@
         <v>5</v>
       </c>
       <c r="K33" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="L33" t="str">
         <f t="shared" ref="L33" si="1">SUBSTITUTE(K33,"skim milk",D33)</f>
-        <v>if (fieldList[158].equals("1")) foods.add("ground beef (75% lean, regular)");</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[158].equals("1")) foods.put("ground beef (75% lean, regular)", 1);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -2261,7 +2260,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -2290,14 +2289,14 @@
         <v>5</v>
       </c>
       <c r="K35" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="L35" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[172].equals("1")) foods.add("hot dog");</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[172].equals("1")) foods.put("hot dog", 1);</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>0</v>
       </c>
@@ -2326,14 +2325,14 @@
         <v>5</v>
       </c>
       <c r="K36" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="L36" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[173].equals("1")) foods.add("hot dog");</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[173].equals("1")) foods.put("hot dog", 1);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -2362,14 +2361,14 @@
         <v>5</v>
       </c>
       <c r="K37" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="L37" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[174].equals("1")) foods.add("low fat hot dog");</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[174].equals("1")) foods.put("low fat hot dog", 1);</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>0</v>
       </c>
@@ -2398,14 +2397,14 @@
         <v>5</v>
       </c>
       <c r="K38" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="L38" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[175].equals("1")) foods.add("hot dog");</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[175].equals("1")) foods.put("hot dog", 1);</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>0</v>
       </c>
@@ -2435,7 +2434,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>0</v>
       </c>
@@ -2464,14 +2463,14 @@
         <v>5</v>
       </c>
       <c r="K40" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="L40" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[205].equals("1")) foods.add("frozen meal");</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[205].equals("1")) foods.put("frozen meal", 1);</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -2500,14 +2499,14 @@
         <v>5</v>
       </c>
       <c r="K41" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="L41" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[206].equals("1")) foods.add("frozen meal");</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[206].equals("1")) foods.put("frozen meal", 1);</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>0</v>
       </c>
@@ -2536,14 +2535,14 @@
         <v>5</v>
       </c>
       <c r="K42" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="L42" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[207].equals("1")) foods.add("frozen meal");</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[207].equals("1")) foods.put("frozen meal", 1);</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>0</v>
       </c>
@@ -2572,14 +2571,14 @@
         <v>5</v>
       </c>
       <c r="K43" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="L43" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[208].equals("1")) foods.add("frozen meal");</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[208].equals("1")) foods.put("frozen meal", 1);</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>0</v>
       </c>
@@ -2609,7 +2608,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -2638,14 +2637,14 @@
         <v>5</v>
       </c>
       <c r="K45" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="L45" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[271].equals("1")) foods.add("bagel");</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[271].equals("1")) foods.put("bagel", 1);</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>0</v>
       </c>
@@ -2674,14 +2673,14 @@
         <v>5</v>
       </c>
       <c r="K46" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="L46" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[272].equals("1")) foods.add("english muffin");</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[272].equals("1")) foods.put("english muffin", 1);</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>0</v>
       </c>
@@ -2710,14 +2709,14 @@
         <v>5</v>
       </c>
       <c r="K47" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="L47" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[273].equals("1")) foods.add("muffin");</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[273].equals("1")) foods.put("muffin", 1);</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>0</v>
       </c>
@@ -2746,14 +2745,14 @@
         <v>5</v>
       </c>
       <c r="K48" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="L48" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[274].equals("1")) foods.add("muffin");</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[274].equals("1")) foods.put("muffin", 1);</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>0</v>
       </c>
@@ -2782,14 +2781,14 @@
         <v>5</v>
       </c>
       <c r="K49" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="L49" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[275].equals("1")) foods.add("danish");</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[275].equals("1")) foods.put("danish", 1);</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>0</v>
       </c>
@@ -2819,7 +2818,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>0</v>
       </c>
@@ -2848,14 +2847,14 @@
         <v>5</v>
       </c>
       <c r="K51" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="L51" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[303].equals("1")) foods.add("soft drink, diet");</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[303].equals("1")) foods.put("soft drink, diet", 1);</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>0</v>
       </c>
@@ -2884,14 +2883,14 @@
         <v>5</v>
       </c>
       <c r="K52" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="L52" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[304].equals("1")) foods.add("soft drink, diet");</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[304].equals("1")) foods.put("soft drink, diet", 1);</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>0</v>
       </c>
@@ -2920,14 +2919,14 @@
         <v>5</v>
       </c>
       <c r="K53" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="L53" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[305].equals("1")) foods.add("soft drink, regular");</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[305].equals("1")) foods.put("soft drink, regular", 1);</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>0</v>
       </c>
@@ -2956,14 +2955,14 @@
         <v>5</v>
       </c>
       <c r="K54" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="L54" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[306].equals("1")) foods.add("soft drink, regular");</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[306].equals("1")) foods.put("soft drink, regular", 1);</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>0</v>
       </c>
@@ -2992,14 +2991,14 @@
         <v>5</v>
       </c>
       <c r="K55" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="L55" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[308].equals("1")) foods.add("100% juice");</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[308].equals("1")) foods.put("100% juice", 1);</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>0</v>
       </c>
@@ -3028,14 +3027,14 @@
         <v>5</v>
       </c>
       <c r="K56" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="L56" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[309].equals("1")) foods.add("juice");</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[309].equals("1")) foods.put("juice", 1);</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>0</v>
       </c>
@@ -3065,7 +3064,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>0</v>
       </c>
@@ -3094,14 +3093,14 @@
         <v>5</v>
       </c>
       <c r="K58" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="L58" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[335].equals("1")) foods.add("whole wheat bread");</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[335].equals("1")) foods.put("whole wheat bread", 1);</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>0</v>
       </c>
@@ -3130,14 +3129,14 @@
         <v>5</v>
       </c>
       <c r="K59" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L59" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[336].equals("1")) foods.add("white bread");</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[336].equals("1")) foods.put("white bread", 1);</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>0</v>
       </c>
@@ -3167,7 +3166,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>0</v>
       </c>
@@ -3196,14 +3195,14 @@
         <v>5</v>
       </c>
       <c r="K61" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="L61" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[347].equals("1")) foods.add("chips");</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[347].equals("1")) foods.put("chips", 1);</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>0</v>
       </c>
@@ -3232,14 +3231,14 @@
         <v>5</v>
       </c>
       <c r="K62" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="L62" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[348].equals("1")) foods.add("chips");</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[348].equals("1")) foods.put("chips", 1);</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>0</v>
       </c>
@@ -3269,7 +3268,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>0</v>
       </c>
@@ -3298,14 +3297,14 @@
         <v>5</v>
       </c>
       <c r="K64" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="L64" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[359].equals("1")) foods.add("cereal");</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[359].equals("1")) foods.put("cereal", 1);</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>0</v>
       </c>
@@ -3334,14 +3333,14 @@
         <v>5</v>
       </c>
       <c r="K65" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="L65" t="str">
         <f t="shared" si="0"/>
-        <v>if (fieldList[360].equals("1")) foods.add("cereal");</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+        <v>if (fieldList[360].equals("1")) foods.put("cereal", 1);</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>0</v>
       </c>

</xml_diff>